<commit_message>
Change .csv and .xlsx
</commit_message>
<xml_diff>
--- a/SCORE-COURSE DATA/filexlsx/courseHK1.xlsx
+++ b/SCORE-COURSE DATA/filexlsx/courseHK1.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\DELL\Desktop\CourseRegistrationSystem_20clc11_4-main\SCORE-COURSE DATA\filexlsx\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AECCDF8D-0817-4945-9A58-29218D6C9973}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CBBAC026-DFFC-4663-B279-54EA28472E04}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1284" yWindow="2292" windowWidth="17280" windowHeight="9036" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -30,9 +30,6 @@
     <t>KTLT</t>
   </si>
   <si>
-    <t>MON</t>
-  </si>
-  <si>
     <t>S1</t>
   </si>
   <si>
@@ -42,9 +39,6 @@
     <t>S4</t>
   </si>
   <si>
-    <t>TUE</t>
-  </si>
-  <si>
     <t xml:space="preserve">CS02			</t>
   </si>
   <si>
@@ -54,24 +48,12 @@
     <t xml:space="preserve">PHY01		</t>
   </si>
   <si>
-    <t xml:space="preserve">	MON</t>
-  </si>
-  <si>
-    <t xml:space="preserve">	S2	</t>
-  </si>
-  <si>
     <t xml:space="preserve">MAT02	</t>
   </si>
   <si>
     <t xml:space="preserve">VTP1B	</t>
   </si>
   <si>
-    <t xml:space="preserve">	S3</t>
-  </si>
-  <si>
-    <t xml:space="preserve">	TUE</t>
-  </si>
-  <si>
     <t xml:space="preserve">MLN01	</t>
   </si>
   <si>
@@ -88,6 +70,24 @@
   </si>
   <si>
     <t>Nguyễn Thanh Phương</t>
+  </si>
+  <si>
+    <t>Sat</t>
+  </si>
+  <si>
+    <t>Wed</t>
+  </si>
+  <si>
+    <t>Mon</t>
+  </si>
+  <si>
+    <t>Tue</t>
+  </si>
+  <si>
+    <t>Fri</t>
+  </si>
+  <si>
+    <t>S3</t>
   </si>
 </sst>
 </file>
@@ -408,25 +408,25 @@
   <dimension ref="A1:I4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A7" sqref="A7:XFD11"/>
+      <selection activeCell="G4" sqref="G4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="45.88671875" customWidth="1"/>
+    <col min="1" max="1" width="8.21875" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="11.33203125" customWidth="1"/>
-    <col min="3" max="3" width="34.5546875" customWidth="1"/>
+    <col min="3" max="3" width="19.88671875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="B1" t="s">
         <v>0</v>
       </c>
       <c r="C1" t="s">
-        <v>18</v>
+        <v>12</v>
       </c>
       <c r="D1">
         <v>4</v>
@@ -435,27 +435,27 @@
         <v>50</v>
       </c>
       <c r="F1" t="s">
+        <v>16</v>
+      </c>
+      <c r="G1" t="s">
         <v>1</v>
       </c>
-      <c r="G1" t="s">
-        <v>2</v>
-      </c>
       <c r="H1" t="s">
-        <v>5</v>
+        <v>15</v>
       </c>
       <c r="I1" t="s">
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="B2" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="C2" t="s">
-        <v>19</v>
+        <v>13</v>
       </c>
       <c r="D2">
         <v>4</v>
@@ -464,27 +464,27 @@
         <v>50</v>
       </c>
       <c r="F2" t="s">
-        <v>9</v>
+        <v>17</v>
       </c>
       <c r="G2" t="s">
-        <v>10</v>
+        <v>1</v>
       </c>
       <c r="H2" t="s">
-        <v>5</v>
+        <v>17</v>
       </c>
       <c r="I2" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
+        <v>7</v>
+      </c>
+      <c r="B3" t="s">
+        <v>8</v>
+      </c>
+      <c r="C3" t="s">
         <v>11</v>
-      </c>
-      <c r="B3" t="s">
-        <v>12</v>
-      </c>
-      <c r="C3" t="s">
-        <v>17</v>
       </c>
       <c r="D3">
         <v>4</v>
@@ -493,45 +493,45 @@
         <v>50</v>
       </c>
       <c r="F3" t="s">
-        <v>1</v>
+        <v>18</v>
       </c>
       <c r="G3" t="s">
-        <v>13</v>
+        <v>2</v>
       </c>
       <c r="H3" t="s">
-        <v>14</v>
+        <v>19</v>
       </c>
       <c r="I3" t="s">
-        <v>13</v>
+        <v>2</v>
       </c>
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
-        <v>15</v>
+        <v>9</v>
       </c>
       <c r="B4" t="s">
-        <v>16</v>
+        <v>10</v>
       </c>
       <c r="C4" t="s">
-        <v>20</v>
+        <v>14</v>
       </c>
       <c r="D4">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="E4">
         <v>50</v>
       </c>
       <c r="F4" t="s">
-        <v>1</v>
+        <v>17</v>
       </c>
       <c r="G4" t="s">
-        <v>4</v>
+        <v>20</v>
       </c>
       <c r="H4" t="s">
-        <v>5</v>
+        <v>17</v>
       </c>
       <c r="I4" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
     </row>
   </sheetData>

</xml_diff>